<commit_message>
headless chrome & multi scenario
</commit_message>
<xml_diff>
--- a/src/main/resources/FootballManagerTesting.xlsx
+++ b/src/main/resources/FootballManagerTesting.xlsx
@@ -4,10 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14115" windowHeight="6870"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14115" windowHeight="6870" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="20">
   <si>
     <t>Result</t>
   </si>
@@ -54,12 +59,6 @@
     <t>confirmPassword</t>
   </si>
   <si>
-    <t>Please fill in all fields</t>
-  </si>
-  <si>
-    <t>Passwords don't match</t>
-  </si>
-  <si>
     <t>email1</t>
   </si>
   <si>
@@ -75,19 +74,16 @@
     <t>email3</t>
   </si>
   <si>
-    <t>User5</t>
-  </si>
-  <si>
-    <t>email5</t>
-  </si>
-  <si>
-    <t>User6</t>
-  </si>
-  <si>
-    <t>email6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Passwords don't match.</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>email4</t>
+  </si>
+  <si>
+    <t>Incomplete fields.</t>
   </si>
 </sst>
 </file>
@@ -441,17 +437,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="31.28515625" customWidth="1" collapsed="1"/>
@@ -486,13 +482,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -503,33 +499,33 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -537,54 +533,340 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" activeCellId="1" sqref="A4:XFD4 A5:XFD5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" activeCellId="3" sqref="A4:XFD4 A5:XFD5 A6:XFD6 A7:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
password match test implemented
</commit_message>
<xml_diff>
--- a/src/main/resources/FootballManagerTesting.xlsx
+++ b/src/main/resources/FootballManagerTesting.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView activeTab="9" windowHeight="6870" windowWidth="14115" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14115" windowHeight="6870"/>
   </bookViews>
   <sheets>
-    <sheet name="Full Input" r:id="rId1" sheetId="1"/>
-    <sheet name="No Name" r:id="rId2" sheetId="2"/>
-    <sheet name="No Email" r:id="rId3" sheetId="3"/>
-    <sheet name="No Pass" r:id="rId4" sheetId="4"/>
-    <sheet name="No Confirm" r:id="rId5" sheetId="5"/>
-    <sheet name="No Input" r:id="rId6" sheetId="6"/>
-    <sheet name="Full Login" r:id="rId7" sheetId="7"/>
-    <sheet name="No Email Login" r:id="rId8" sheetId="8"/>
-    <sheet name="No Pass Login" r:id="rId9" sheetId="9"/>
-    <sheet name="No Input Login" r:id="rId10" sheetId="10"/>
+    <sheet name="Create Full Input" sheetId="1" r:id="rId1"/>
+    <sheet name="Create No Name" sheetId="2" r:id="rId2"/>
+    <sheet name="Create No Email" sheetId="3" r:id="rId3"/>
+    <sheet name="Create No Pass" sheetId="4" r:id="rId4"/>
+    <sheet name="Create No Confirm" sheetId="5" r:id="rId5"/>
+    <sheet name="Create No Input" sheetId="6" r:id="rId6"/>
+    <sheet name="Login Full" sheetId="7" r:id="rId7"/>
+    <sheet name="Login No Email" sheetId="8" r:id="rId8"/>
+    <sheet name="Login No Pass" sheetId="9" r:id="rId9"/>
+    <sheet name="Login No Input" sheetId="10" r:id="rId10"/>
+    <sheet name="Create Pass Match" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="24">
   <si>
     <t>Result</t>
   </si>
@@ -97,13 +98,15 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>Passwords don’t match</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,14 +141,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -171,10 +174,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -193,10 +196,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -231,7 +234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -266,7 +269,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -360,21 +363,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -391,7 +394,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -443,29 +446,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -525,70 +528,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -613,13 +570,106 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -627,10 +677,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -694,13 +744,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D3"/>
@@ -708,12 +758,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -777,13 +826,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D3"/>
@@ -791,10 +840,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -858,26 +906,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -911,7 +958,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -931,7 +978,7 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
@@ -941,13 +988,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -955,7 +1002,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="1" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -992,13 +1039,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1006,8 +1053,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,13 +1097,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1064,8 +1111,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1099,13 +1146,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1113,8 +1160,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1148,6 +1195,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated constants and ids
</commit_message>
<xml_diff>
--- a/src/main/resources/FootballManagerTesting.xlsx
+++ b/src/main/resources/FootballManagerTesting.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView activeTab="12" firstSheet="5" windowHeight="6870" windowWidth="14115" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14115" windowHeight="6870" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="Create Full Input" r:id="rId1" sheetId="1"/>
-    <sheet name="Create No Name" r:id="rId2" sheetId="2"/>
-    <sheet name="Create No Email" r:id="rId3" sheetId="3"/>
-    <sheet name="Create No Pass" r:id="rId4" sheetId="4"/>
-    <sheet name="Create No Confirm" r:id="rId5" sheetId="5"/>
-    <sheet name="Create No Input" r:id="rId6" sheetId="6"/>
-    <sheet name="Login Full" r:id="rId7" sheetId="7"/>
-    <sheet name="Login No Email" r:id="rId8" sheetId="8"/>
-    <sheet name="Login No Pass" r:id="rId9" sheetId="9"/>
-    <sheet name="Login No Input" r:id="rId10" sheetId="10"/>
-    <sheet name="Create Pass Match" r:id="rId11" sheetId="11"/>
-    <sheet name="List Join" r:id="rId12" sheetId="12"/>
-    <sheet name="List Remove" r:id="rId13" sheetId="13"/>
+    <sheet name="Create Full Input" sheetId="1" r:id="rId1"/>
+    <sheet name="Create No Name" sheetId="2" r:id="rId2"/>
+    <sheet name="Create No Email" sheetId="3" r:id="rId3"/>
+    <sheet name="Create No Pass" sheetId="4" r:id="rId4"/>
+    <sheet name="Create No Confirm" sheetId="5" r:id="rId5"/>
+    <sheet name="Create No Input" sheetId="6" r:id="rId6"/>
+    <sheet name="Login Full" sheetId="7" r:id="rId7"/>
+    <sheet name="Login No Email" sheetId="8" r:id="rId8"/>
+    <sheet name="Login No Pass" sheetId="9" r:id="rId9"/>
+    <sheet name="Login No Input" sheetId="10" r:id="rId10"/>
+    <sheet name="Create Pass Match" sheetId="11" r:id="rId11"/>
+    <sheet name="List Join" sheetId="12" r:id="rId12"/>
+    <sheet name="List Remove" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="21">
   <si>
     <t>Result</t>
   </si>
@@ -93,14 +93,13 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>Monday Night Football Squad</t>
+    <t>Here is a list of everyone that has been added already</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,14 +134,14 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -168,10 +167,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -190,10 +189,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -228,7 +227,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -263,7 +262,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -357,21 +356,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -388,7 +387,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -440,29 +439,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -523,14 +522,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
@@ -538,8 +537,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,13 +563,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -578,13 +577,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="31.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -657,13 +656,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -671,12 +670,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -737,26 +736,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -817,13 +816,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -831,10 +830,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -898,13 +897,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -912,11 +911,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -980,13 +979,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D3"/>
@@ -994,9 +993,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1060,13 +1059,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
@@ -1074,11 +1073,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1142,13 +1141,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -1156,7 +1155,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="1" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,22 +1192,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1251,13 +1250,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1265,8 +1264,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,13 +1299,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1314,8 +1313,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1349,6 +1348,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>